<commit_message>
Adicion de servicios HELP y modificacion a funcion de cargar servicios
</commit_message>
<xml_diff>
--- a/CATEDRA/catalogocatedra.xlsx
+++ b/CATEDRA/catalogocatedra.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GEEO\GEEO-WebApp\media\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GEEO\GEEO-WebApp\CATEDRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="295">
   <si>
     <r>
       <rPr>
@@ -1505,6 +1506,396 @@
       </rPr>
       <t>scaffolding</t>
     </r>
+  </si>
+  <si>
+    <t>Alternativas de transición a post escuela</t>
+  </si>
+  <si>
+    <t>Ahora viene lo mejor! Herramientas para una transición positiva</t>
+  </si>
+  <si>
+    <t>Mapa de Ruta al éxito postsecundario</t>
+  </si>
+  <si>
+    <t>Un camino de triunfo para mi hijo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apoyo a la adquisición de idiomas  </t>
+  </si>
+  <si>
+    <t>Konesans se pouvwa (Conocimiento es poder) Lo que el saber otras lenguas puede hacer por tu hijo/a</t>
+  </si>
+  <si>
+    <t>Apoyo a la transición escolar y ambientes nuevos</t>
+  </si>
+  <si>
+    <t>Las transiciones… el pan nuestro de cada día</t>
+  </si>
+  <si>
+    <t>Preparación para la escuela y las transiciones</t>
+  </si>
+  <si>
+    <t>La transición escolar y la maravilla de descubrir nuevas posibilidades</t>
+  </si>
+  <si>
+    <t>Cómo desarrollar buenos hábitos de estudio</t>
+  </si>
+  <si>
+    <t>Cómo preparamos a nuestros hijos a tener buenos hábitos de estudio?</t>
+  </si>
+  <si>
+    <t>Eb= Em. Estudiar bien es igual a ejecutar mejor: el desarrollo de hábitos de estudio</t>
+  </si>
+  <si>
+    <t>Plan de estudio de mi hijo</t>
+  </si>
+  <si>
+    <t>Cómo desarrollar buenos hábitos de estudio. Apoyo a la adquisición de idiomas</t>
+  </si>
+  <si>
+    <t>Explorando la tecnología de videojuegos controlados por la mente</t>
+  </si>
+  <si>
+    <t>Cómo interpretar exámenes y el informe de rendimiento académico. Cómo monitorear el progreso del estudiante</t>
+  </si>
+  <si>
+    <t>Entendiendo tu esfuerzo: lo que me hablas a través de tus calificaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cómo monitorear el progreso del estudiante </t>
+  </si>
+  <si>
+    <t>Siguiendo el camino correcto: mis oportunidades para monitorear el progreso de mi hijo/a</t>
+  </si>
+  <si>
+    <t>Cómo promover la lectura en el hogar</t>
+  </si>
+  <si>
+    <t>Círculos literarios para padres</t>
+  </si>
+  <si>
+    <t>La magia de la escritura</t>
+  </si>
+  <si>
+    <t>Maneras sencillas de ayudar a desarrollar la lectura en mis hijos desde su nacimiento</t>
+  </si>
+  <si>
+    <t>Si leemos, entendemos: el arte de la lectura en el ambiente hogareño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cómo promover la lectura en el hogar. Apoyo a la adquisición de idiomas </t>
+  </si>
+  <si>
+    <t>Mi nene lee…pero no entiende lo que lee. La importancia de la comprensión lectora en el aprovechamiento académico de mi hijo, de mi nieto.</t>
+  </si>
+  <si>
+    <t>Comunicación efectiva</t>
+  </si>
+  <si>
+    <t>Mis padres discuten constantemente: pensamientos de un hijo (a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunicación efectiva. Promoción de valores en el hogar </t>
+  </si>
+  <si>
+    <t>El juego simbólico como campo de aprendizaje – Enfoque Sistémico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunicación efectiva. Técnicas para el manejo de la crianza </t>
+  </si>
+  <si>
+    <t>El arte, el cerebro y nuestros pensamientos”</t>
+  </si>
+  <si>
+    <t>La experiencia de comunicarte hábilmente con tu hijo y su relación en su desempeño escolar</t>
+  </si>
+  <si>
+    <t>Comunicación Efectiva. Apoyo a la transición</t>
+  </si>
+  <si>
+    <t>Comunicación efectiva. Cómo monitorear el progreso del estudiante</t>
+  </si>
+  <si>
+    <t>Escuchando lo que no se dice</t>
+  </si>
+  <si>
+    <t>Comunicación efectiva. Promoción de valores en el hogar</t>
+  </si>
+  <si>
+    <t>Comunicación efectiva entre miembros del “equipo invencible”</t>
+  </si>
+  <si>
+    <t>Comunicación efectiva. Técnicas de disciplina positiva. Promoción de valores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grupo de apoyo- Compartiendo experiencias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curso de contenido de idioma </t>
+  </si>
+  <si>
+    <t>Desde aquí hasta el infinito: el panorama universal ante el dominio de idiomas</t>
+  </si>
+  <si>
+    <t>Establecer y mantener redes de apoyo en la comunidad</t>
+  </si>
+  <si>
+    <t>Aplicación práctica de la Pedagogía Sistémica en el escenario familiar</t>
+  </si>
+  <si>
+    <t>El padre como gestor de la escuela para mejorar el aprovechamiento de su hijo.</t>
+  </si>
+  <si>
+    <t>La biblioteca pública de mi pueblo… cómo me puede ayudar en la educación de mi hijo.</t>
+  </si>
+  <si>
+    <t>Mi comunidad…mi gran aliado</t>
+  </si>
+  <si>
+    <t>Explicando la Carta Circular de participación de padres</t>
+  </si>
+  <si>
+    <t>Establecer y mantener redes de apoyo en la comunidad. Liderazgo. Cómo monitorear el progreso del estudiante.</t>
+  </si>
+  <si>
+    <t>A decir presente y a participar!</t>
+  </si>
+  <si>
+    <t>Factores de riesgo y prevención</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factores de riesgo y prevención </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factores de riesgo y prevención  </t>
+  </si>
+  <si>
+    <t>Cómo trabajar para tener hijos menos violentos y agresivos</t>
+  </si>
+  <si>
+    <t>Conociendo los rasgos de personalidad de mi hijo (a) para optimizar la comunicación</t>
+  </si>
+  <si>
+    <t>La inteligencia emocional y sus implicaciones en el éxito de vida de mi hijo</t>
+  </si>
+  <si>
+    <t>Las redes sociales en el entorno de mi hijo</t>
+  </si>
+  <si>
+    <t>Prevención de Violencia Doméstica</t>
+  </si>
+  <si>
+    <t>Resiliencia ¿Cómo lograr la excelencia en el lugar de trabajo?</t>
+  </si>
+  <si>
+    <t>Protegiendo mi semilla</t>
+  </si>
+  <si>
+    <t>Cómo se lo explico a mi hijo?</t>
+  </si>
+  <si>
+    <t>Factores de riesgo y prevención. Comunicación efectiva.</t>
+  </si>
+  <si>
+    <t>Está bien!… “Si no se siente bien”</t>
+  </si>
+  <si>
+    <t>Los sentimientos de mi hijo</t>
+  </si>
+  <si>
+    <t>Factores de riesgo y prevención. Leyes que protegen la niñez (Educación Especial, “cyberbullying”, etc.).</t>
+  </si>
+  <si>
+    <t>Acoso escolar, “Bullying”</t>
+  </si>
+  <si>
+    <t>Leyes que protegen la niñez (Educación Especial, “cyberbullying”, etc.).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El derecho a mi favor: leyes que protegen a mis hijos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El derecho penal como respuesta a la actividad delictiva </t>
+  </si>
+  <si>
+    <t>Liderazgo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liderazgo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promoviendo la responsabilidad y autonomía de mi hijo </t>
+  </si>
+  <si>
+    <t>El líder que hay en ti: alcanzando la plenitud mediante el ejercicio del liderazgo</t>
+  </si>
+  <si>
+    <t>Mediación de conflictos. Comunicación efectiva</t>
+  </si>
+  <si>
+    <t>Conflictos: Oportunidades para conocer y crecer.</t>
+  </si>
+  <si>
+    <t>Ese conflicto… tema superado. Cómo trabajar adecuadamente las situaciones conflictivas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mediación de conflictos. Promoción de valores en el hogar. Factores de riesgo y prevención </t>
+  </si>
+  <si>
+    <t>Manejo adecuado de conflictos</t>
+  </si>
+  <si>
+    <t>Navegando el  sistema  educativo. Cómo monitorear el progreso del estudiante.</t>
+  </si>
+  <si>
+    <t>Sistema educativo: un mar que debo navegar</t>
+  </si>
+  <si>
+    <t>Navegando el sistema educativo</t>
+  </si>
+  <si>
+    <t>Navegando en la página del Departamento de Educación</t>
+  </si>
+  <si>
+    <t>Navegando el sistema educativo. Cómo monitorear el progreso del estudiante.</t>
+  </si>
+  <si>
+    <t>Sistema de Información Estudiantil (SIE)</t>
+  </si>
+  <si>
+    <t>Preparación. Motivación en la participación de las pruebas del estado. Cómo desarrollar buenos hábitos de estudio.</t>
+  </si>
+  <si>
+    <t>Tu logro es el mío! Preparándote para dar el máximo en las pruebas</t>
+  </si>
+  <si>
+    <t>Promoción de valores en el hogar</t>
+  </si>
+  <si>
+    <t>Autogestión: Bisutería, Diseño y Creación de “Choker”</t>
+  </si>
+  <si>
+    <t>Biografía de mi corazón!</t>
+  </si>
+  <si>
+    <t>Las competencias educativas a través de una mirada sistémica</t>
+  </si>
+  <si>
+    <t>Manejo de la sala de clases a través de valores</t>
+  </si>
+  <si>
+    <t>Presupuesto familiar:  equilibrio entre el dar y el tomar</t>
+  </si>
+  <si>
+    <t>Promoción de valores en el hogar. Comunicación efectiva.</t>
+  </si>
+  <si>
+    <t>Presente en su Presente”</t>
+  </si>
+  <si>
+    <t>Mi sistema de valores: la transmisión de valores positivos en el hogar</t>
+  </si>
+  <si>
+    <t>Respetando y aceptando la diversidad</t>
+  </si>
+  <si>
+    <t>Valores:  la llave del éxito en la vida</t>
+  </si>
+  <si>
+    <t>Técnica para el manejo de la crianza en las etapas de desarrollo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La familia como primera escuela de mi hijo </t>
+  </si>
+  <si>
+    <t>Técnicas de disciplina positiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuáles son las necesidades reales de mis hijos y cómo saberlo?    </t>
+  </si>
+  <si>
+    <t>Técnicas de disciplina positiva. Comunicación efectiva.</t>
+  </si>
+  <si>
+    <t>El arte de construir con amor</t>
+  </si>
+  <si>
+    <t>Técnicas de disciplina positiva. Comunicación efectiva. Promoción de valores.</t>
+  </si>
+  <si>
+    <t>Manejo de emociones desde la neurociencia</t>
+  </si>
+  <si>
+    <t>Técnicas de disciplina positiva. Promoción de valores en el hogar.</t>
+  </si>
+  <si>
+    <t>Del Padre que soy al Padre que quiero ser.</t>
+  </si>
+  <si>
+    <t>Técnicas de disciplina positiva. Promoción de valores en el hogar. Comunicación efectiva.</t>
+  </si>
+  <si>
+    <t>Disciplina con amor</t>
+  </si>
+  <si>
+    <t>Técnicas para el manejo de crianza en las etapas de desarrollo</t>
+  </si>
+  <si>
+    <t>Te entiendo! Es cuestión del desarrollo….</t>
+  </si>
+  <si>
+    <t>Técnicas para el manejo de crianza en las etapas de desarrollo. Comunicación efectiva.</t>
+  </si>
+  <si>
+    <t>La Adolescencia”</t>
+  </si>
+  <si>
+    <t>La crianza compartida, una alternativa necesaria para la educación de nuestros hijos</t>
+  </si>
+  <si>
+    <t>Técnicas para el manejo de crianza en las etapas de desarrollo. Técnicas para promover la salud, la nutrición y una vida activa de los (as) estudiantes</t>
+  </si>
+  <si>
+    <t>Creciendo y aprendiendo en familia!</t>
+  </si>
+  <si>
+    <t>Técnicas para el manejo de la crianza en las etapas de desarrollo</t>
+  </si>
+  <si>
+    <t>Soy abuelo criando nietos: “necesito herramientas para ayudarlos a estudiar”</t>
+  </si>
+  <si>
+    <t>Técnicas para promover la salud, la nutrición y una vida activa de los (as) estudiantes</t>
+  </si>
+  <si>
+    <t>Actívate, muévete y disfruta de lo saludable previniendo el sobrepeso y obesidad</t>
+  </si>
+  <si>
+    <t>Alimentación sana, mente sana”</t>
+  </si>
+  <si>
+    <t>Lee las etiquetas nutricionales y aprende a seleccionar meriendas saludables</t>
+  </si>
+  <si>
+    <t>Promoviendo una excelente nutrición: “Mi Plato para un Puerto Rico Saludable”</t>
+  </si>
+  <si>
+    <t>Técnicas para promover la salud, la nutrición y una vida activa de los estudiantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La salud del estudiante, trabajo de todos </t>
+  </si>
+  <si>
+    <t>La salud, la buena alimentación y la vida activa como elementos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temas de cultura puertorriqueña </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cultura y esencia: el arte de ser puertorriqueño </t>
+  </si>
+  <si>
+    <t>HELP</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1985,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1606,6 +1997,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1888,7 +2282,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3505,4 +3901,914 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="134.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>294</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>294</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>294</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>294</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>294</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>294</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C35" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>294</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C37" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C38" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>294</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C40" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>294</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>294</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>294</v>
+      </c>
+      <c r="B43" t="s">
+        <v>230</v>
+      </c>
+      <c r="C43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>294</v>
+      </c>
+      <c r="B44" t="s">
+        <v>232</v>
+      </c>
+      <c r="C44" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>294</v>
+      </c>
+      <c r="B45" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>294</v>
+      </c>
+      <c r="B46" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>294</v>
+      </c>
+      <c r="B47" t="s">
+        <v>236</v>
+      </c>
+      <c r="C47" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>294</v>
+      </c>
+      <c r="B48" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>294</v>
+      </c>
+      <c r="B49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>294</v>
+      </c>
+      <c r="B50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
+        <v>244</v>
+      </c>
+      <c r="C51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>294</v>
+      </c>
+      <c r="B52" t="s">
+        <v>246</v>
+      </c>
+      <c r="C52" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>294</v>
+      </c>
+      <c r="B53" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>294</v>
+      </c>
+      <c r="B54" t="s">
+        <v>250</v>
+      </c>
+      <c r="C54" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>294</v>
+      </c>
+      <c r="B55" t="s">
+        <v>252</v>
+      </c>
+      <c r="C55" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>294</v>
+      </c>
+      <c r="B56" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>294</v>
+      </c>
+      <c r="B57" t="s">
+        <v>252</v>
+      </c>
+      <c r="C57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>294</v>
+      </c>
+      <c r="B58" t="s">
+        <v>252</v>
+      </c>
+      <c r="C58" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>294</v>
+      </c>
+      <c r="B59" t="s">
+        <v>252</v>
+      </c>
+      <c r="C59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>294</v>
+      </c>
+      <c r="B60" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>294</v>
+      </c>
+      <c r="B61" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>294</v>
+      </c>
+      <c r="B62" t="s">
+        <v>258</v>
+      </c>
+      <c r="C62" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>294</v>
+      </c>
+      <c r="B63" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>294</v>
+      </c>
+      <c r="B64" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>294</v>
+      </c>
+      <c r="B65" t="s">
+        <v>265</v>
+      </c>
+      <c r="C65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>294</v>
+      </c>
+      <c r="B66" t="s">
+        <v>267</v>
+      </c>
+      <c r="C66" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>294</v>
+      </c>
+      <c r="B67" t="s">
+        <v>269</v>
+      </c>
+      <c r="C67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>294</v>
+      </c>
+      <c r="B68" t="s">
+        <v>271</v>
+      </c>
+      <c r="C68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>294</v>
+      </c>
+      <c r="B69" t="s">
+        <v>273</v>
+      </c>
+      <c r="C69" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>294</v>
+      </c>
+      <c r="B70" t="s">
+        <v>275</v>
+      </c>
+      <c r="C70" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>294</v>
+      </c>
+      <c r="B71" t="s">
+        <v>277</v>
+      </c>
+      <c r="C71" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>294</v>
+      </c>
+      <c r="B72" t="s">
+        <v>277</v>
+      </c>
+      <c r="C72" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>294</v>
+      </c>
+      <c r="B73" t="s">
+        <v>280</v>
+      </c>
+      <c r="C73" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>294</v>
+      </c>
+      <c r="B74" t="s">
+        <v>282</v>
+      </c>
+      <c r="C74" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" t="s">
+        <v>284</v>
+      </c>
+      <c r="C75" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>294</v>
+      </c>
+      <c r="B76" t="s">
+        <v>284</v>
+      </c>
+      <c r="C76" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>294</v>
+      </c>
+      <c r="B77" t="s">
+        <v>284</v>
+      </c>
+      <c r="C77" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>294</v>
+      </c>
+      <c r="B78" t="s">
+        <v>284</v>
+      </c>
+      <c r="C78" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>294</v>
+      </c>
+      <c r="B79" t="s">
+        <v>289</v>
+      </c>
+      <c r="C79" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>294</v>
+      </c>
+      <c r="B80" t="s">
+        <v>289</v>
+      </c>
+      <c r="C80" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>294</v>
+      </c>
+      <c r="B81" t="s">
+        <v>292</v>
+      </c>
+      <c r="C81" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>